<commit_message>
microthermometry and new EOS
</commit_message>
<xml_diff>
--- a/Benchmarking/CO2_Homogenization_Temps/Batch_processing_TC.xlsx
+++ b/Benchmarking/CO2_Homogenization_Temps/Batch_processing_TC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\Benchmarking\CO2_Homogenization_Temps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6254C765-9F8D-4FD0-B846-91097E52D85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7F05E6-5EE3-43DA-A417-D3052A0046DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{9022BC05-3138-46E6-A3AD-C82E9882530C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{9022BC05-3138-46E6-A3AD-C82E9882530C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40BA542-111E-4D70-AA24-C87BFDFA8D30}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,7 +462,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>-4</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-5</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>-1.2</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>0.3</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>4.5</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>25</v>
+        <v>-10</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>31</v>
+        <v>-15</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>-50</v>
+        <v>-20</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>-5.6</v>
+        <v>-25</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>-5.5</v>
+        <v>-30</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>-5.6</v>
+        <v>-35</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>

</xml_diff>